<commit_message>
done with prokect 2 written work
</commit_message>
<xml_diff>
--- a/WrittenWork/ProperParseTable.xlsx
+++ b/WrittenWork/ProperParseTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelcollett/Compilerv2/Compiler/WrittenWork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{974F24E1-760A-F44F-BEFC-7C0F9D8F678C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538D1615-5DC5-DF4F-BBF1-31A21CFBC0E7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{A079371B-9211-CA4F-995E-1B1981D0C497}"/>
+    <workbookView xWindow="14900" yWindow="0" windowWidth="13900" windowHeight="18000" xr2:uid="{A079371B-9211-CA4F-995E-1B1981D0C497}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,358 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>program’</t>
+  </si>
+  <si>
+    <t>program’’</t>
+  </si>
+  <si>
+    <t>idlst</t>
+  </si>
+  <si>
+    <t>idlst’</t>
+  </si>
+  <si>
+    <t>declarations</t>
+  </si>
+  <si>
+    <t>declarations’</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>standard_type</t>
+  </si>
+  <si>
+    <t>subdeclarations</t>
+  </si>
+  <si>
+    <t>subdeclarations’</t>
+  </si>
+  <si>
+    <t>subdeclaration</t>
+  </si>
+  <si>
+    <t>subdeclaration’</t>
+  </si>
+  <si>
+    <t>subdeclaration’’</t>
+  </si>
+  <si>
+    <t>subprogram_head</t>
+  </si>
+  <si>
+    <t>subprogram_head’</t>
+  </si>
+  <si>
+    <t>arguments</t>
+  </si>
+  <si>
+    <t>parameter_list</t>
+  </si>
+  <si>
+    <t>parameter_list’</t>
+  </si>
+  <si>
+    <t>compound_statement</t>
+  </si>
+  <si>
+    <t>compound_statement’</t>
+  </si>
+  <si>
+    <t>optional_statements</t>
+  </si>
+  <si>
+    <t>statement_list</t>
+  </si>
+  <si>
+    <t>statement_list’</t>
+  </si>
+  <si>
+    <t>statement</t>
+  </si>
+  <si>
+    <t>statement’</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>variable’</t>
+  </si>
+  <si>
+    <t>procedure_statement</t>
+  </si>
+  <si>
+    <t>procedure_statement’</t>
+  </si>
+  <si>
+    <t>expression_list</t>
+  </si>
+  <si>
+    <t>expression_list’</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>expression’</t>
+  </si>
+  <si>
+    <t>simple_expression</t>
+  </si>
+  <si>
+    <t>simple_expression’</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>term’</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>factor’</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>procedure</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>assignop</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>relop</t>
+  </si>
+  <si>
+    <t>addop</t>
+  </si>
+  <si>
+    <t>mulop</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>6.2.1</t>
+  </si>
+  <si>
+    <t>6.2.2</t>
+  </si>
+  <si>
+    <t>7.2.1</t>
+  </si>
+  <si>
+    <t>7.2.2</t>
+  </si>
+  <si>
+    <t>7.2.3</t>
+  </si>
+  <si>
+    <t>7.3.1</t>
+  </si>
+  <si>
+    <t>7.3.2</t>
+  </si>
+  <si>
+    <t>8.2.1</t>
+  </si>
+  <si>
+    <t>8.2.2</t>
+  </si>
+  <si>
+    <t>10.2.1</t>
+  </si>
+  <si>
+    <t>10.2.2</t>
+  </si>
+  <si>
+    <t>11.2.1</t>
+  </si>
+  <si>
+    <t>11.2.2</t>
+  </si>
+  <si>
+    <t>13.2.1</t>
+  </si>
+  <si>
+    <t>13.2.2</t>
+  </si>
+  <si>
+    <t>14.6.2</t>
+  </si>
+  <si>
+    <t>14.6.1</t>
+  </si>
+  <si>
+    <t>15.2.1</t>
+  </si>
+  <si>
+    <t>15.2.2</t>
+  </si>
+  <si>
+    <t>16.2.1</t>
+  </si>
+  <si>
+    <t>16.2.2</t>
+  </si>
+  <si>
+    <t>17.2.1</t>
+  </si>
+  <si>
+    <t>17.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.2.1 </t>
+  </si>
+  <si>
+    <t>18.2.2</t>
+  </si>
+  <si>
+    <t>19.3.1</t>
+  </si>
+  <si>
+    <t>19.3.2</t>
+  </si>
+  <si>
+    <t>20.2.1</t>
+  </si>
+  <si>
+    <t>20.2.2</t>
+  </si>
+  <si>
+    <t>21.5.1</t>
+  </si>
+  <si>
+    <t>21.5.2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +403,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +723,735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C37F2B-E7C5-794E-BB33-A09CA2EA42D0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>4.2</v>
+      </c>
+      <c r="I9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J9">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J10">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z18">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="L22" t="s">
+        <v>89</v>
+      </c>
+      <c r="M22" t="s">
+        <v>90</v>
+      </c>
+      <c r="O22" t="s">
+        <v>89</v>
+      </c>
+      <c r="R22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>12.1</v>
+      </c>
+      <c r="L23">
+        <v>12.1</v>
+      </c>
+      <c r="O23">
+        <v>12.1</v>
+      </c>
+      <c r="R23">
+        <v>12.1</v>
+      </c>
+      <c r="AD23">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>13.1</v>
+      </c>
+      <c r="L24">
+        <v>13.1</v>
+      </c>
+      <c r="O24">
+        <v>13.1</v>
+      </c>
+      <c r="R24">
+        <v>13.1</v>
+      </c>
+      <c r="AD24">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>14.1</v>
+      </c>
+      <c r="L26">
+        <v>14.3</v>
+      </c>
+      <c r="O26">
+        <v>14.5</v>
+      </c>
+      <c r="R26">
+        <v>14.4</v>
+      </c>
+      <c r="AD26">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+      <c r="M27" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD30">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="M31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="H32">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="W32">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="X32">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="Y32">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="Z32">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="H34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="W34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="X34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="Y34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="Z34">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="M35" t="s">
+        <v>102</v>
+      </c>
+      <c r="P35" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>102</v>
+      </c>
+      <c r="S35" t="s">
+        <v>102</v>
+      </c>
+      <c r="T35" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H36">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="W36">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="X36">
+        <v>19.2</v>
+      </c>
+      <c r="Y36">
+        <v>19.2</v>
+      </c>
+      <c r="Z36">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="M37" t="s">
+        <v>104</v>
+      </c>
+      <c r="P37" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>104</v>
+      </c>
+      <c r="S37" t="s">
+        <v>104</v>
+      </c>
+      <c r="T37" t="s">
+        <v>104</v>
+      </c>
+      <c r="U37" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="H38">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="W38">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Z38">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="M39" t="s">
+        <v>106</v>
+      </c>
+      <c r="P39" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>106</v>
+      </c>
+      <c r="S39" t="s">
+        <v>106</v>
+      </c>
+      <c r="T39" t="s">
+        <v>106</v>
+      </c>
+      <c r="U39" t="s">
+        <v>106</v>
+      </c>
+      <c r="V39" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>21.1</v>
+      </c>
+      <c r="H40">
+        <v>21.2</v>
+      </c>
+      <c r="W40">
+        <v>21.4</v>
+      </c>
+      <c r="Z40">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+      <c r="M41" t="s">
+        <v>108</v>
+      </c>
+      <c r="P41" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>108</v>
+      </c>
+      <c r="S41" t="s">
+        <v>108</v>
+      </c>
+      <c r="T41" t="s">
+        <v>108</v>
+      </c>
+      <c r="U41" t="s">
+        <v>108</v>
+      </c>
+      <c r="V41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X42">
+        <v>22.1</v>
+      </c>
+      <c r="Y42">
+        <v>22.2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>